<commit_message>
changed and updated site area measurements
</commit_message>
<xml_diff>
--- a/input/Pheromone_trap_moth_counts9.xlsx
+++ b/input/Pheromone_trap_moth_counts9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Noa/Documents/Documents - MacBook Air/PhD/R:Stats:GIS/RStudio/R_Workspace/Pheromone_trap_code/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A44735-9DB0-3243-BF54-73CD23EB69CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A8E99B-3B89-7548-ABB2-74CB1014C186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28400" windowHeight="15800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28400" windowHeight="15800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1529,10 +1529,10 @@
     <t>VIN-even</t>
   </si>
   <si>
-    <t>Patch Size (km2)</t>
-  </si>
-  <si>
-    <t>Extracted by drawing a polygon inclusive of all traps within a patch (on Google maps)</t>
+    <t>Forest Area (km2)</t>
+  </si>
+  <si>
+    <t>Area of continuous forest within which each patch is found - drawing a polygon in Google Maps, boundaries determined by the presence of urban development/agricultural fields/highways</t>
   </si>
 </sst>
 </file>
@@ -12058,7 +12058,7 @@
       </c>
       <c r="O3" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>78.231658657067996</v>
+        <v>67.203417636614247</v>
       </c>
       <c r="P3" s="29" t="s">
         <v>249</v>
@@ -12072,7 +12072,7 @@
       </c>
       <c r="S3" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>117.481658657068</v>
+        <v>106.45341763661425</v>
       </c>
       <c r="V3" s="5" t="s">
         <v>178</v>
@@ -12188,7 +12188,7 @@
       </c>
       <c r="O5" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>75.199239003739535</v>
+        <v>53.223267762261997</v>
       </c>
       <c r="P5" s="29" t="s">
         <v>248</v>
@@ -12202,7 +12202,7 @@
       </c>
       <c r="S5" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>128.69923900373954</v>
+        <v>106.723267762262</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>176</v>
@@ -12251,7 +12251,7 @@
       </c>
       <c r="O6" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>95.642219231604031</v>
+        <v>84.469373727903189</v>
       </c>
       <c r="P6" s="29" t="s">
         <v>248</v>
@@ -12265,7 +12265,7 @@
       </c>
       <c r="S6" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>95.642219231604031</v>
+        <v>84.469373727903189</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>53</v>
@@ -12322,7 +12322,7 @@
       </c>
       <c r="O7" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>73.450342985955615</v>
+        <v>63.567734835994862</v>
       </c>
       <c r="P7" s="29" t="s">
         <v>249</v>
@@ -12336,7 +12336,7 @@
       </c>
       <c r="S7" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>111.45034298595561</v>
+        <v>101.56773483599486</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>180</v>
@@ -12874,7 +12874,7 @@
       </c>
       <c r="O16" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>6.4430426177553572</v>
+        <v>14.130266039700501</v>
       </c>
       <c r="P16" s="26" t="s">
         <v>250</v>
@@ -12888,7 +12888,7 @@
       </c>
       <c r="S16" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>52.69304261775536</v>
+        <v>60.380266039700501</v>
       </c>
       <c r="V16" s="5" t="s">
         <v>195</v>
@@ -12942,7 +12942,7 @@
       </c>
       <c r="O17" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>18.928025987248386</v>
+        <v>12.529713375086347</v>
       </c>
       <c r="P17" s="26" t="s">
         <v>249</v>
@@ -12956,7 +12956,7 @@
       </c>
       <c r="S17" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>69.92802598724839</v>
+        <v>63.529713375086345</v>
       </c>
       <c r="T17" s="5" t="s">
         <v>201</v>
@@ -12998,7 +12998,7 @@
       </c>
       <c r="O18" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>76.453698818257294</v>
+        <v>71.638242168492965</v>
       </c>
       <c r="P18" s="39" t="s">
         <v>249</v>
@@ -13012,7 +13012,7 @@
       </c>
       <c r="S18" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>76.453698818257294</v>
+        <v>71.638242168492965</v>
       </c>
       <c r="V18" s="5" t="s">
         <v>199</v>
@@ -13122,7 +13122,7 @@
       </c>
       <c r="O20" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>16.677471535901095</v>
+        <v>3.6827641923858403</v>
       </c>
       <c r="P20" s="26" t="s">
         <v>250</v>
@@ -13136,7 +13136,7 @@
       </c>
       <c r="S20" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>41.927471535901091</v>
+        <v>28.932764192385839</v>
       </c>
       <c r="T20" s="5" t="s">
         <v>43</v>
@@ -13193,7 +13193,7 @@
       </c>
       <c r="O21" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>5.0640020058220561</v>
+        <v>12.620061304756483</v>
       </c>
       <c r="P21" s="26" t="s">
         <v>252</v>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="S21" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>20.564002005822054</v>
+        <v>28.120061304756483</v>
       </c>
       <c r="V21" s="5" t="s">
         <v>13</v>
@@ -13379,7 +13379,7 @@
       </c>
       <c r="O24" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>15.161635094686487</v>
+        <v>3.888534895634967</v>
       </c>
       <c r="P24" s="26" t="s">
         <v>250</v>
@@ -13393,7 +13393,7 @@
       </c>
       <c r="S24" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>55.661635094686488</v>
+        <v>44.388534895634969</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -13559,7 +13559,7 @@
       </c>
       <c r="O27" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>43.264709021331171</v>
+        <v>26.126722448115355</v>
       </c>
       <c r="P27" s="29" t="s">
         <v>250</v>
@@ -13573,7 +13573,7 @@
       </c>
       <c r="S27" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>61.764709021331171</v>
+        <v>44.626722448115359</v>
       </c>
       <c r="T27" s="5" t="s">
         <v>164</v>
@@ -13630,7 +13630,7 @@
       </c>
       <c r="O28" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>59.552322082949871</v>
+        <v>58.403004980615279</v>
       </c>
       <c r="P28" s="29" t="s">
         <v>249</v>
@@ -13644,7 +13644,7 @@
       </c>
       <c r="S28" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>95.552322082949871</v>
+        <v>94.403004980615279</v>
       </c>
       <c r="T28" s="5" t="s">
         <v>154</v>
@@ -13763,7 +13763,7 @@
       </c>
       <c r="O30" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>107.52859457336618</v>
+        <v>118.85879820662313</v>
       </c>
       <c r="P30" s="29" t="s">
         <v>249</v>
@@ -13777,7 +13777,7 @@
       </c>
       <c r="S30" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>114.52859457336618</v>
+        <v>125.85879820662313</v>
       </c>
       <c r="T30" s="26" t="s">
         <v>240</v>
@@ -14235,7 +14235,7 @@
       </c>
       <c r="O38" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>14.306847667219122</v>
+        <v>1.641164580221234</v>
       </c>
       <c r="P38" s="28" t="s">
         <v>250</v>
@@ -14249,7 +14249,7 @@
       </c>
       <c r="S38" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>41.806847667219124</v>
+        <v>29.141164580221233</v>
       </c>
       <c r="T38" s="12"/>
       <c r="U38" s="12"/>
@@ -14363,7 +14363,7 @@
       </c>
       <c r="O40" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>109.27446526749907</v>
+        <v>96.744268046576749</v>
       </c>
       <c r="P40" s="29" t="s">
         <v>248</v>
@@ -14377,7 +14377,7 @@
       </c>
       <c r="S40" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>109.27446526749907</v>
+        <v>96.744268046576749</v>
       </c>
       <c r="V40" s="5" t="s">
         <v>99</v>
@@ -14426,7 +14426,7 @@
       </c>
       <c r="O41" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>95.742155861852993</v>
+        <v>82.571059574011542</v>
       </c>
       <c r="P41" s="29" t="s">
         <v>248</v>
@@ -14440,7 +14440,7 @@
       </c>
       <c r="S41" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>95.742155861852993</v>
+        <v>82.571059574011542</v>
       </c>
       <c r="V41" s="5" t="s">
         <v>99</v>
@@ -14668,7 +14668,7 @@
       </c>
       <c r="O45" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>5.792034707166958</v>
+        <v>12.436926071290788</v>
       </c>
       <c r="P45" s="26" t="s">
         <v>252</v>
@@ -14682,7 +14682,7 @@
       </c>
       <c r="S45" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>12.292034707166959</v>
+        <v>18.936926071290788</v>
       </c>
       <c r="V45" s="5" t="s">
         <v>74</v>
@@ -14795,7 +14795,7 @@
       </c>
       <c r="O47" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>70.048213731704436</v>
+        <v>72.165949977612968</v>
       </c>
       <c r="P47" s="29" t="s">
         <v>249</v>
@@ -14809,7 +14809,7 @@
       </c>
       <c r="S47" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>101.04821373170444</v>
+        <v>103.16594997761297</v>
       </c>
       <c r="U47" s="5" t="s">
         <v>70</v>
@@ -14925,7 +14925,7 @@
       </c>
       <c r="O49" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>27.631036322498034</v>
+        <v>23.981617655691771</v>
       </c>
       <c r="P49" s="29" t="s">
         <v>250</v>
@@ -14939,7 +14939,7 @@
       </c>
       <c r="S49" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>27.631036322498034</v>
+        <v>23.981617655691771</v>
       </c>
       <c r="V49" s="5" t="s">
         <v>77</v>
@@ -15100,7 +15100,7 @@
       </c>
       <c r="O52" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>117.13454995298935</v>
+        <v>81.494764375428886</v>
       </c>
       <c r="P52" s="29" t="s">
         <v>248</v>
@@ -15114,7 +15114,7 @@
       </c>
       <c r="S52" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>117.13454995298935</v>
+        <v>81.494764375428886</v>
       </c>
       <c r="V52" s="5" t="s">
         <v>80</v>
@@ -15163,7 +15163,7 @@
       </c>
       <c r="O53" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>91.524544964327106</v>
+        <v>88.886805922624191</v>
       </c>
       <c r="P53" s="29" t="s">
         <v>248</v>
@@ -15177,7 +15177,7 @@
       </c>
       <c r="S53" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>91.524544964327106</v>
+        <v>88.886805922624191</v>
       </c>
       <c r="V53" s="5" t="s">
         <v>84</v>
@@ -15344,7 +15344,7 @@
       </c>
       <c r="O56" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>74.946142415690147</v>
+        <v>50.56702479591177</v>
       </c>
       <c r="P56" t="s">
         <v>249</v>
@@ -15358,7 +15358,7 @@
       </c>
       <c r="S56" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>74.946142415690147</v>
+        <v>50.56702479591177</v>
       </c>
       <c r="V56" s="5" t="s">
         <v>209</v>
@@ -15407,7 +15407,7 @@
       </c>
       <c r="O57" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>113.03554201126065</v>
+        <v>86.046435609242096</v>
       </c>
       <c r="P57" s="29" t="s">
         <v>248</v>
@@ -15421,7 +15421,7 @@
       </c>
       <c r="S57" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>113.03554201126065</v>
+        <v>86.046435609242096</v>
       </c>
       <c r="V57" s="5" t="s">
         <v>214</v>
@@ -15529,7 +15529,7 @@
       </c>
       <c r="O59" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>114.09155279387419</v>
+        <v>96.179181244734949</v>
       </c>
       <c r="P59" s="29" t="s">
         <v>248</v>
@@ -15543,7 +15543,7 @@
       </c>
       <c r="S59" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>114.09155279387419</v>
+        <v>96.179181244734949</v>
       </c>
       <c r="V59" s="5" t="s">
         <v>212</v>
@@ -15707,7 +15707,7 @@
       </c>
       <c r="O62" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>113.94630053303572</v>
+        <v>81.421466542120442</v>
       </c>
       <c r="P62" s="29" t="s">
         <v>248</v>
@@ -15721,7 +15721,7 @@
       </c>
       <c r="S62" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>113.94630053303572</v>
+        <v>81.421466542120442</v>
       </c>
       <c r="V62" s="5" t="s">
         <v>174</v>
@@ -15770,7 +15770,7 @@
       </c>
       <c r="O63" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>108.73970466962709</v>
+        <v>97.424583702026453</v>
       </c>
       <c r="P63" s="29" t="s">
         <v>248</v>
@@ -15784,7 +15784,7 @@
       </c>
       <c r="S63" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>108.73970466962709</v>
+        <v>97.424583702026453</v>
       </c>
       <c r="V63" s="5" t="s">
         <v>174</v>
@@ -15880,7 +15880,7 @@
       </c>
       <c r="O65" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>100.88418923084778</v>
+        <v>84.512259224537004</v>
       </c>
       <c r="P65" s="29" t="s">
         <v>248</v>
@@ -15894,7 +15894,7 @@
       </c>
       <c r="S65" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>100.88418923084778</v>
+        <v>84.512259224537004</v>
       </c>
       <c r="V65" s="5" t="s">
         <v>189</v>
@@ -15943,7 +15943,7 @@
       </c>
       <c r="O66" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>100.91383633320386</v>
+        <v>118.28094238489547</v>
       </c>
       <c r="P66" s="29" t="s">
         <v>248</v>
@@ -15957,7 +15957,7 @@
       </c>
       <c r="S66" s="36">
         <f t="shared" ref="S66:S97" ca="1" si="11">J66+O66</f>
-        <v>100.91383633320386</v>
+        <v>118.28094238489547</v>
       </c>
       <c r="V66" s="5" t="s">
         <v>174</v>
@@ -16121,7 +16121,7 @@
       </c>
       <c r="O69" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>109.31293462008512</v>
+        <v>97.667467450852769</v>
       </c>
       <c r="P69" s="29" t="s">
         <v>248</v>
@@ -16135,7 +16135,7 @@
       </c>
       <c r="S69" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>109.31293462008512</v>
+        <v>97.667467450852769</v>
       </c>
       <c r="V69" s="5" t="s">
         <v>229</v>
@@ -16251,7 +16251,7 @@
       </c>
       <c r="O71" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>25.002709322219673</v>
+        <v>39.66301561182194</v>
       </c>
       <c r="P71" s="29" t="s">
         <v>250</v>
@@ -16265,7 +16265,7 @@
       </c>
       <c r="S71" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>34.002709322219673</v>
+        <v>48.66301561182194</v>
       </c>
       <c r="V71" s="5" t="s">
         <v>226</v>
@@ -16322,7 +16322,7 @@
       </c>
       <c r="O72" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>70.991015735575203</v>
+        <v>72.08713506824904</v>
       </c>
       <c r="P72" s="29" t="s">
         <v>249</v>
@@ -16336,7 +16336,7 @@
       </c>
       <c r="S72" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>100.4910157355752</v>
+        <v>101.58713506824904</v>
       </c>
       <c r="V72" s="5" t="s">
         <v>223</v>
@@ -16388,7 +16388,7 @@
       </c>
       <c r="O73" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>99.89189083509018</v>
+        <v>95.609596350325575</v>
       </c>
       <c r="P73" s="29" t="s">
         <v>248</v>
@@ -16402,7 +16402,7 @@
       </c>
       <c r="S73" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>99.89189083509018</v>
+        <v>95.609596350325575</v>
       </c>
       <c r="V73" s="5" t="s">
         <v>229</v>
@@ -16699,7 +16699,7 @@
       </c>
       <c r="O78" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>4.1534772687983885</v>
+        <v>0.27216380642122173</v>
       </c>
       <c r="P78" s="39" t="s">
         <v>248</v>
@@ -16713,7 +16713,7 @@
       </c>
       <c r="S78" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>84.903477268798383</v>
+        <v>81.022163806421219</v>
       </c>
       <c r="V78" s="5" t="s">
         <v>113</v>
@@ -16770,7 +16770,7 @@
       </c>
       <c r="O79" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>10.309566454689127</v>
+        <v>13.423219221272504</v>
       </c>
       <c r="P79" s="26" t="s">
         <v>249</v>
@@ -16784,7 +16784,7 @@
       </c>
       <c r="S79" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>68.059566454689133</v>
+        <v>71.173219221272504</v>
       </c>
       <c r="T79" s="5" t="s">
         <v>120</v>
@@ -16901,7 +16901,7 @@
       </c>
       <c r="O81" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>20.751968159395823</v>
+        <v>24.033943709628794</v>
       </c>
       <c r="P81" s="29" t="s">
         <v>248</v>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="S81" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>80.00196815939583</v>
+        <v>83.283943709628801</v>
       </c>
       <c r="V81" s="5" t="s">
         <v>18</v>
@@ -17266,7 +17266,7 @@
       </c>
       <c r="O87" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>72.52749005265683</v>
+        <v>51.387828304790766</v>
       </c>
       <c r="P87" s="29" t="s">
         <v>249</v>
@@ -17280,7 +17280,7 @@
       </c>
       <c r="S87" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>106.77749005265683</v>
+        <v>85.637828304790759</v>
       </c>
       <c r="T87" s="5">
         <v>0</v>
@@ -17400,7 +17400,7 @@
       </c>
       <c r="O89" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>3.8632019608248194</v>
+        <v>16.136566022367504</v>
       </c>
       <c r="P89" s="27" t="s">
         <v>249</v>
@@ -17414,7 +17414,7 @@
       </c>
       <c r="S89" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>54.613201960824817</v>
+        <v>66.886566022367504</v>
       </c>
       <c r="T89" s="26" t="s">
         <v>235</v>
@@ -17537,7 +17537,7 @@
       </c>
       <c r="O91" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>15.367027541707001</v>
+        <v>16.281900427577465</v>
       </c>
       <c r="P91" s="26" t="s">
         <v>250</v>
@@ -17551,7 +17551,7 @@
       </c>
       <c r="S91" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>47.617027541707003</v>
+        <v>48.531900427577469</v>
       </c>
       <c r="T91" s="5" t="s">
         <v>37</v>
@@ -17842,7 +17842,7 @@
       </c>
       <c r="O96" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>114.22941398061909</v>
+        <v>88.804307183449851</v>
       </c>
       <c r="P96" s="29" t="s">
         <v>248</v>
@@ -17856,7 +17856,7 @@
       </c>
       <c r="S96" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>114.22941398061909</v>
+        <v>88.804307183449851</v>
       </c>
       <c r="V96" s="5" t="s">
         <v>145</v>
@@ -17913,7 +17913,7 @@
       </c>
       <c r="O97" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>83.591189445581151</v>
+        <v>80.670274127465916</v>
       </c>
       <c r="P97" s="29" t="s">
         <v>248</v>
@@ -17927,7 +17927,7 @@
       </c>
       <c r="S97" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>124.59118944558115</v>
+        <v>121.67027412746592</v>
       </c>
       <c r="V97" s="5" t="s">
         <v>145</v>
@@ -18046,7 +18046,7 @@
       </c>
       <c r="O99" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>53.292989468934977</v>
+        <v>59.457220473601602</v>
       </c>
       <c r="P99" s="29" t="s">
         <v>248</v>
@@ -18060,7 +18060,7 @@
       </c>
       <c r="S99" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>117.54298946893498</v>
+        <v>123.70722047360161</v>
       </c>
       <c r="T99" s="5" t="s">
         <v>133</v>
@@ -18176,7 +18176,7 @@
       </c>
       <c r="O101" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>45.642512949553961</v>
+        <v>26.88645365179736</v>
       </c>
       <c r="P101" s="29" t="s">
         <v>250</v>
@@ -18190,7 +18190,7 @@
       </c>
       <c r="S101" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>53.642512949553961</v>
+        <v>34.88645365179736</v>
       </c>
       <c r="T101" s="26" t="s">
         <v>239</v>
@@ -18315,7 +18315,7 @@
       </c>
       <c r="O103" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>0.9485989085989831</v>
+        <v>8.9751082051278814</v>
       </c>
       <c r="P103" s="26" t="s">
         <v>250</v>
@@ -18329,7 +18329,7 @@
       </c>
       <c r="S103" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>41.198598908598981</v>
+        <v>49.225108205127881</v>
       </c>
       <c r="T103" s="5" t="s">
         <v>137</v>
@@ -21698,11 +21698,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E8C7F5-2756-2840-8463-9090EA3CE12E}">
   <dimension ref="A1:V119"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="96" workbookViewId="0">
       <pane xSplit="11" ySplit="16" topLeftCell="P17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="D68" sqref="D68:D73"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -21806,7 +21806,7 @@
         <v>171</v>
       </c>
       <c r="D2" s="73">
-        <v>0.67</v>
+        <v>1282</v>
       </c>
       <c r="E2" s="73">
         <v>28.25</v>
@@ -21868,7 +21868,7 @@
         <v>177</v>
       </c>
       <c r="D3" s="73">
-        <v>0.67</v>
+        <v>1282</v>
       </c>
       <c r="E3" s="73">
         <v>39.25</v>
@@ -21933,7 +21933,7 @@
         <v>168</v>
       </c>
       <c r="D4" s="73">
-        <v>0.67</v>
+        <v>1282</v>
       </c>
       <c r="E4" s="73">
         <v>33.75</v>
@@ -21995,7 +21995,7 @@
         <v>175</v>
       </c>
       <c r="D5" s="73">
-        <v>0.67</v>
+        <v>1282</v>
       </c>
       <c r="E5" s="73">
         <v>53.5</v>
@@ -22060,7 +22060,7 @@
         <v>173</v>
       </c>
       <c r="D6" s="73">
-        <v>0.67</v>
+        <v>1282</v>
       </c>
       <c r="F6" s="49" t="s">
         <v>76</v>
@@ -22122,7 +22122,7 @@
         <v>179</v>
       </c>
       <c r="D7" s="73">
-        <v>0.67</v>
+        <v>1282</v>
       </c>
       <c r="E7" s="73">
         <v>38</v>
@@ -22187,7 +22187,7 @@
         <v>52</v>
       </c>
       <c r="D8" s="73">
-        <v>0.16700000000000001</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E8" s="73">
         <v>83</v>
@@ -22249,7 +22249,7 @@
         <v>61</v>
       </c>
       <c r="D9" s="73">
-        <v>0.16700000000000001</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E9" s="73">
         <v>91.25</v>
@@ -22311,7 +22311,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="73">
-        <v>0.16700000000000001</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E10" s="73">
         <v>40</v>
@@ -22373,7 +22373,7 @@
         <v>58</v>
       </c>
       <c r="D11" s="73">
-        <v>0.16700000000000001</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E11" s="73">
         <v>86</v>
@@ -22435,7 +22435,7 @@
         <v>54</v>
       </c>
       <c r="D12" s="73">
-        <v>0.16700000000000001</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E12" s="73">
         <v>71.25</v>
@@ -22494,7 +22494,7 @@
         <v>63</v>
       </c>
       <c r="D13" s="73">
-        <v>0.16700000000000001</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E13" s="73">
         <v>77.25</v>
@@ -22553,7 +22553,7 @@
         <v>196</v>
       </c>
       <c r="D14" s="73">
-        <v>15.1</v>
+        <v>1282</v>
       </c>
       <c r="E14" s="73">
         <v>5.25</v>
@@ -22615,7 +22615,7 @@
         <v>203</v>
       </c>
       <c r="D15" s="73">
-        <v>15.1</v>
+        <v>1282</v>
       </c>
       <c r="E15" s="73">
         <v>16.75</v>
@@ -22677,7 +22677,7 @@
         <v>194</v>
       </c>
       <c r="D16" s="73">
-        <v>15.1</v>
+        <v>1282</v>
       </c>
       <c r="E16" s="73">
         <v>46.25</v>
@@ -22742,7 +22742,7 @@
         <v>200</v>
       </c>
       <c r="D17" s="73">
-        <v>15.1</v>
+        <v>1282</v>
       </c>
       <c r="E17" s="73">
         <v>51</v>
@@ -22807,7 +22807,7 @@
         <v>198</v>
       </c>
       <c r="D18" s="73">
-        <v>15.1</v>
+        <v>1282</v>
       </c>
       <c r="F18" s="49" t="s">
         <v>76</v>
@@ -22863,7 +22863,7 @@
         <v>204</v>
       </c>
       <c r="D19" s="73">
-        <v>15.1</v>
+        <v>1282</v>
       </c>
       <c r="E19" s="73">
         <v>15</v>
@@ -22922,7 +22922,7 @@
         <v>42</v>
       </c>
       <c r="D20" s="73">
-        <v>0.13800000000000001</v>
+        <v>73.3</v>
       </c>
       <c r="E20" s="73">
         <v>25.25</v>
@@ -22987,7 +22987,7 @@
         <v>47</v>
       </c>
       <c r="D21" s="73">
-        <v>0.13800000000000001</v>
+        <v>73.3</v>
       </c>
       <c r="E21" s="73">
         <v>15.5</v>
@@ -23052,7 +23052,7 @@
         <v>41</v>
       </c>
       <c r="D22" s="73">
-        <v>0.13800000000000001</v>
+        <v>73.3</v>
       </c>
       <c r="E22" s="73">
         <v>35.25</v>
@@ -23114,7 +23114,7 @@
         <v>45</v>
       </c>
       <c r="D23" s="73">
-        <v>0.13800000000000001</v>
+        <v>73.3</v>
       </c>
       <c r="E23" s="73">
         <v>42</v>
@@ -23176,7 +23176,7 @@
         <v>44</v>
       </c>
       <c r="D24" s="73">
-        <v>0.13800000000000001</v>
+        <v>73.3</v>
       </c>
       <c r="E24" s="73">
         <v>40.5</v>
@@ -23238,7 +23238,7 @@
         <v>48</v>
       </c>
       <c r="D25" s="73">
-        <v>0.13800000000000001</v>
+        <v>73.3</v>
       </c>
       <c r="E25" s="73">
         <v>46</v>
@@ -23298,7 +23298,7 @@
         <v>157</v>
       </c>
       <c r="D26" s="73">
-        <v>0.372</v>
+        <v>44.4</v>
       </c>
       <c r="E26" s="73">
         <v>35</v>
@@ -23360,7 +23360,7 @@
         <v>163</v>
       </c>
       <c r="D27" s="73">
-        <v>0.372</v>
+        <v>44.4</v>
       </c>
       <c r="E27" s="73">
         <v>18.5</v>
@@ -23428,7 +23428,7 @@
         <v>153</v>
       </c>
       <c r="D28" s="73">
-        <v>0.372</v>
+        <v>44.4</v>
       </c>
       <c r="E28" s="73">
         <v>36</v>
@@ -23493,7 +23493,7 @@
         <v>161</v>
       </c>
       <c r="D29" s="73">
-        <v>0.372</v>
+        <v>44.4</v>
       </c>
       <c r="E29" s="73">
         <v>41</v>
@@ -23558,7 +23558,7 @@
         <v>158</v>
       </c>
       <c r="D30" s="73">
-        <v>0.372</v>
+        <v>44.4</v>
       </c>
       <c r="E30" s="73">
         <v>7</v>
@@ -23620,7 +23620,7 @@
         <v>166</v>
       </c>
       <c r="D31" s="73">
-        <v>0.372</v>
+        <v>44.4</v>
       </c>
       <c r="E31" s="73">
         <v>8.5</v>
@@ -23682,7 +23682,7 @@
         <v>91</v>
       </c>
       <c r="D32" s="73">
-        <v>0.76300000000000001</v>
+        <v>14</v>
       </c>
       <c r="E32" s="73">
         <v>33</v>
@@ -23744,7 +23744,7 @@
         <v>95</v>
       </c>
       <c r="D33" s="73">
-        <v>0.76300000000000001</v>
+        <v>14</v>
       </c>
       <c r="E33" s="73">
         <v>6.25</v>
@@ -23806,7 +23806,7 @@
         <v>90</v>
       </c>
       <c r="D34" s="73">
-        <v>0.76300000000000001</v>
+        <v>14</v>
       </c>
       <c r="E34" s="73">
         <v>21</v>
@@ -23868,7 +23868,7 @@
         <v>94</v>
       </c>
       <c r="D35" s="73">
-        <v>0.76300000000000001</v>
+        <v>14</v>
       </c>
       <c r="E35" s="73">
         <v>42.75</v>
@@ -23930,7 +23930,7 @@
         <v>93</v>
       </c>
       <c r="D36" s="73">
-        <v>0.76300000000000001</v>
+        <v>14</v>
       </c>
       <c r="E36" s="73">
         <v>18.5</v>
@@ -23989,7 +23989,7 @@
         <v>96</v>
       </c>
       <c r="D37" s="73">
-        <v>0.76300000000000001</v>
+        <v>14</v>
       </c>
       <c r="E37" s="73">
         <v>9</v>
@@ -24048,7 +24048,7 @@
         <v>100</v>
       </c>
       <c r="D38" s="73">
-        <v>0.62</v>
+        <v>14</v>
       </c>
       <c r="E38" s="73">
         <v>27.5</v>
@@ -24113,7 +24113,7 @@
         <v>105</v>
       </c>
       <c r="D39" s="73">
-        <v>0.62</v>
+        <v>14</v>
       </c>
       <c r="E39" s="73">
         <v>13</v>
@@ -24175,7 +24175,7 @@
         <v>98</v>
       </c>
       <c r="D40" s="73">
-        <v>0.62</v>
+        <v>14</v>
       </c>
       <c r="F40" s="49" t="s">
         <v>76</v>
@@ -24237,7 +24237,7 @@
         <v>104</v>
       </c>
       <c r="D41" s="73">
-        <v>0.62</v>
+        <v>14</v>
       </c>
       <c r="F41" s="49" t="s">
         <v>76</v>
@@ -24299,7 +24299,7 @@
         <v>103</v>
       </c>
       <c r="D42" s="73">
-        <v>0.62</v>
+        <v>14</v>
       </c>
       <c r="E42" s="73">
         <v>28</v>
@@ -24361,7 +24361,7 @@
         <v>106</v>
       </c>
       <c r="D43" s="73">
-        <v>0.62</v>
+        <v>14</v>
       </c>
       <c r="E43" s="73">
         <v>48</v>
@@ -24420,7 +24420,7 @@
         <v>67</v>
       </c>
       <c r="D44" s="73">
-        <v>0.3</v>
+        <v>12.4</v>
       </c>
       <c r="E44" s="73">
         <v>6.5</v>
@@ -24482,7 +24482,7 @@
         <v>73</v>
       </c>
       <c r="D45" s="73">
-        <v>0.3</v>
+        <v>12.4</v>
       </c>
       <c r="E45" s="73">
         <v>6.5</v>
@@ -24547,7 +24547,7 @@
         <v>66</v>
       </c>
       <c r="D46" s="73">
-        <v>0.3</v>
+        <v>12.4</v>
       </c>
       <c r="E46" s="73">
         <v>26.75</v>
@@ -24609,7 +24609,7 @@
         <v>69</v>
       </c>
       <c r="D47" s="73">
-        <v>0.3</v>
+        <v>12.4</v>
       </c>
       <c r="E47" s="73">
         <v>31</v>
@@ -24674,7 +24674,7 @@
         <v>68</v>
       </c>
       <c r="D48" s="73">
-        <v>0.3</v>
+        <v>12.4</v>
       </c>
       <c r="E48" s="73">
         <v>12.25</v>
@@ -24734,7 +24734,7 @@
         <v>75</v>
       </c>
       <c r="D49" s="73">
-        <v>0.3</v>
+        <v>12.4</v>
       </c>
       <c r="E49" s="73">
         <v>0</v>
@@ -24796,7 +24796,7 @@
         <v>81</v>
       </c>
       <c r="D50" s="73">
-        <v>0.40200000000000002</v>
+        <v>12.4</v>
       </c>
       <c r="E50" s="73">
         <v>9</v>
@@ -24861,7 +24861,7 @@
         <v>85</v>
       </c>
       <c r="D51" s="73">
-        <v>0.40200000000000002</v>
+        <v>12.4</v>
       </c>
       <c r="E51" s="73">
         <v>27.25</v>
@@ -24926,7 +24926,7 @@
         <v>79</v>
       </c>
       <c r="D52" s="73">
-        <v>0.40200000000000002</v>
+        <v>12.4</v>
       </c>
       <c r="F52" s="49" t="s">
         <v>76</v>
@@ -24988,7 +24988,7 @@
         <v>83</v>
       </c>
       <c r="D53" s="73">
-        <v>0.40200000000000002</v>
+        <v>12.4</v>
       </c>
       <c r="F53" s="49" t="s">
         <v>76</v>
@@ -25050,7 +25050,7 @@
         <v>82</v>
       </c>
       <c r="D54" s="73">
-        <v>0.40200000000000002</v>
+        <v>12.4</v>
       </c>
       <c r="E54" s="73">
         <v>1</v>
@@ -25109,7 +25109,7 @@
         <v>86</v>
       </c>
       <c r="D55" s="73">
-        <v>0.40200000000000002</v>
+        <v>12.4</v>
       </c>
       <c r="E55" s="73">
         <v>0</v>
@@ -25168,7 +25168,7 @@
         <v>208</v>
       </c>
       <c r="D56" s="73">
-        <v>0.113</v>
+        <v>16.3</v>
       </c>
       <c r="F56" s="49" t="s">
         <v>76</v>
@@ -25230,7 +25230,7 @@
         <v>213</v>
       </c>
       <c r="D57" s="73">
-        <v>0.113</v>
+        <v>16.3</v>
       </c>
       <c r="F57" s="49" t="s">
         <v>76</v>
@@ -25292,7 +25292,7 @@
         <v>206</v>
       </c>
       <c r="D58" s="73">
-        <v>0.113</v>
+        <v>16.3</v>
       </c>
       <c r="E58" s="73">
         <v>0</v>
@@ -25354,7 +25354,7 @@
         <v>211</v>
       </c>
       <c r="D59" s="73">
-        <v>0.113</v>
+        <v>16.3</v>
       </c>
       <c r="F59" s="49" t="s">
         <v>76</v>
@@ -25416,7 +25416,7 @@
         <v>210</v>
       </c>
       <c r="D60" s="73">
-        <v>0.113</v>
+        <v>16.3</v>
       </c>
       <c r="E60" s="73">
         <v>2</v>
@@ -25478,7 +25478,7 @@
         <v>215</v>
       </c>
       <c r="D61" s="73">
-        <v>0.113</v>
+        <v>16.3</v>
       </c>
       <c r="E61" s="73">
         <v>33</v>
@@ -25540,7 +25540,7 @@
         <v>186</v>
       </c>
       <c r="D62" s="73">
-        <v>0.433</v>
+        <v>1282</v>
       </c>
       <c r="F62" s="49" t="s">
         <v>76</v>
@@ -25602,7 +25602,7 @@
         <v>190</v>
       </c>
       <c r="D63" s="73">
-        <v>0.433</v>
+        <v>1282</v>
       </c>
       <c r="F63" s="49" t="s">
         <v>76</v>
@@ -25667,7 +25667,7 @@
         <v>184</v>
       </c>
       <c r="D64" s="73">
-        <v>0.433</v>
+        <v>1282</v>
       </c>
       <c r="E64" s="73">
         <v>0</v>
@@ -25726,7 +25726,7 @@
         <v>188</v>
       </c>
       <c r="D65" s="73">
-        <v>0.433</v>
+        <v>1282</v>
       </c>
       <c r="F65" s="49" t="s">
         <v>76</v>
@@ -25785,7 +25785,7 @@
         <v>187</v>
       </c>
       <c r="D66" s="73">
-        <v>0.433</v>
+        <v>1282</v>
       </c>
       <c r="F66" s="49" t="s">
         <v>76</v>
@@ -25844,7 +25844,7 @@
         <v>191</v>
       </c>
       <c r="D67" s="73">
-        <v>0.433</v>
+        <v>1282</v>
       </c>
       <c r="E67" s="73">
         <v>43.25</v>
@@ -25900,7 +25900,7 @@
         <v>220</v>
       </c>
       <c r="D68" s="73">
-        <v>0.84899999999999998</v>
+        <v>2.17</v>
       </c>
       <c r="E68" s="73">
         <v>30</v>
@@ -25962,7 +25962,7 @@
         <v>228</v>
       </c>
       <c r="D69" s="73">
-        <v>0.84899999999999998</v>
+        <v>2.17</v>
       </c>
       <c r="F69" s="49" t="s">
         <v>76</v>
@@ -26024,7 +26024,7 @@
         <v>217</v>
       </c>
       <c r="D70" s="73">
-        <v>0.84899999999999998</v>
+        <v>2.17</v>
       </c>
       <c r="E70" s="73">
         <v>86.25</v>
@@ -26086,7 +26086,7 @@
         <v>225</v>
       </c>
       <c r="D71" s="73">
-        <v>0.84899999999999998</v>
+        <v>2.17</v>
       </c>
       <c r="E71" s="73">
         <v>9</v>
@@ -26151,7 +26151,7 @@
         <v>222</v>
       </c>
       <c r="D72" s="73">
-        <v>0.84899999999999998</v>
+        <v>2.17</v>
       </c>
       <c r="E72" s="73">
         <v>29.5</v>
@@ -26219,7 +26219,7 @@
         <v>230</v>
       </c>
       <c r="D73" s="73">
-        <v>0.84899999999999998</v>
+        <v>2.17</v>
       </c>
       <c r="F73" s="49" t="s">
         <v>76</v>
@@ -26284,7 +26284,7 @@
         <v>110</v>
       </c>
       <c r="D74" s="73">
-        <v>1.36</v>
+        <v>1.59</v>
       </c>
       <c r="E74" s="73">
         <v>78</v>
@@ -26346,7 +26346,7 @@
         <v>117</v>
       </c>
       <c r="D75" s="73">
-        <v>1.36</v>
+        <v>1.59</v>
       </c>
       <c r="E75" s="73">
         <v>68.25</v>
@@ -26408,7 +26408,7 @@
         <v>108</v>
       </c>
       <c r="D76" s="73">
-        <v>1.36</v>
+        <v>1.59</v>
       </c>
       <c r="E76" s="73">
         <v>92.5</v>
@@ -26470,7 +26470,7 @@
         <v>115</v>
       </c>
       <c r="D77" s="73">
-        <v>1.36</v>
+        <v>1.59</v>
       </c>
       <c r="E77" s="73">
         <v>44</v>
@@ -26532,7 +26532,7 @@
         <v>112</v>
       </c>
       <c r="D78" s="73">
-        <v>1.36</v>
+        <v>1.59</v>
       </c>
       <c r="E78" s="73">
         <v>80.75</v>
@@ -26597,7 +26597,7 @@
         <v>119</v>
       </c>
       <c r="D79" s="73">
-        <v>1.36</v>
+        <v>1.59</v>
       </c>
       <c r="E79" s="73">
         <v>57.75</v>
@@ -26662,7 +26662,7 @@
         <v>11</v>
       </c>
       <c r="D80" s="73">
-        <v>1.2</v>
+        <v>108</v>
       </c>
       <c r="E80" s="73">
         <v>81.75</v>
@@ -26724,7 +26724,7 @@
         <v>17</v>
       </c>
       <c r="D81" s="73">
-        <v>1.2</v>
+        <v>108</v>
       </c>
       <c r="E81" s="73">
         <v>59.25</v>
@@ -26789,7 +26789,7 @@
         <v>8</v>
       </c>
       <c r="D82" s="73">
-        <v>1.2</v>
+        <v>108</v>
       </c>
       <c r="E82" s="73">
         <v>53</v>
@@ -26851,7 +26851,7 @@
         <v>15</v>
       </c>
       <c r="D83" s="73">
-        <v>1.2</v>
+        <v>108</v>
       </c>
       <c r="E83" s="73">
         <v>50.5</v>
@@ -26913,7 +26913,7 @@
         <v>14</v>
       </c>
       <c r="D84" s="73">
-        <v>1.2</v>
+        <v>108</v>
       </c>
       <c r="E84" s="73">
         <v>54.25</v>
@@ -26972,7 +26972,7 @@
         <v>19</v>
       </c>
       <c r="D85" s="73">
-        <v>1.2</v>
+        <v>108</v>
       </c>
       <c r="E85" s="73">
         <v>55.25</v>
@@ -27034,7 +27034,7 @@
         <v>26</v>
       </c>
       <c r="D86" s="73">
-        <v>0.65700000000000003</v>
+        <v>108</v>
       </c>
       <c r="E86" s="73">
         <v>62.75</v>
@@ -27096,7 +27096,7 @@
         <v>34</v>
       </c>
       <c r="D87" s="73">
-        <v>0.65700000000000003</v>
+        <v>108</v>
       </c>
       <c r="E87" s="73">
         <v>34.25</v>
@@ -27161,7 +27161,7 @@
         <v>23</v>
       </c>
       <c r="D88" s="73">
-        <v>0.65700000000000003</v>
+        <v>108</v>
       </c>
       <c r="E88" s="73">
         <v>76</v>
@@ -27226,7 +27226,7 @@
         <v>31</v>
       </c>
       <c r="D89" s="73">
-        <v>0.65700000000000003</v>
+        <v>108</v>
       </c>
       <c r="E89" s="73">
         <v>50.75</v>
@@ -27294,7 +27294,7 @@
         <v>29</v>
       </c>
       <c r="D90" s="73">
-        <v>0.65700000000000003</v>
+        <v>108</v>
       </c>
       <c r="E90" s="73">
         <v>18.25</v>
@@ -27353,7 +27353,7 @@
         <v>36</v>
       </c>
       <c r="D91" s="73">
-        <v>0.65700000000000003</v>
+        <v>108</v>
       </c>
       <c r="E91" s="73">
         <v>32.25</v>
@@ -27415,7 +27415,7 @@
         <v>141</v>
       </c>
       <c r="D92" s="73">
-        <v>0.81499999999999995</v>
+        <v>12.3</v>
       </c>
       <c r="E92" s="73">
         <v>77.25</v>
@@ -27480,7 +27480,7 @@
         <v>148</v>
       </c>
       <c r="D93" s="73">
-        <v>0.81499999999999995</v>
+        <v>12.3</v>
       </c>
       <c r="E93" s="73">
         <v>49.5</v>
@@ -27545,7 +27545,7 @@
         <v>140</v>
       </c>
       <c r="D94" s="73">
-        <v>0.81499999999999995</v>
+        <v>12.3</v>
       </c>
       <c r="E94" s="73">
         <v>68</v>
@@ -27610,7 +27610,7 @@
         <v>147</v>
       </c>
       <c r="D95" s="73">
-        <v>0.81499999999999995</v>
+        <v>12.3</v>
       </c>
       <c r="E95" s="73">
         <v>79.25</v>
@@ -27675,7 +27675,7 @@
         <v>144</v>
       </c>
       <c r="D96" s="73">
-        <v>0.81499999999999995</v>
+        <v>12.3</v>
       </c>
       <c r="F96" s="49" t="s">
         <v>76</v>
@@ -27740,7 +27740,7 @@
         <v>150</v>
       </c>
       <c r="D97" s="73">
-        <v>0.81499999999999995</v>
+        <v>12.3</v>
       </c>
       <c r="E97" s="73">
         <v>41</v>
@@ -27808,7 +27808,7 @@
         <v>123</v>
       </c>
       <c r="D98" s="83">
-        <v>0.79300000000000004</v>
+        <v>2.72</v>
       </c>
       <c r="E98" s="73">
         <v>97.5</v>
@@ -27870,7 +27870,7 @@
         <v>132</v>
       </c>
       <c r="D99" s="83">
-        <v>0.79300000000000004</v>
+        <v>2.72</v>
       </c>
       <c r="E99" s="73">
         <v>64.25</v>
@@ -27935,7 +27935,7 @@
         <v>122</v>
       </c>
       <c r="D100" s="83">
-        <v>0.79300000000000004</v>
+        <v>2.72</v>
       </c>
       <c r="E100" s="73">
         <v>29</v>
@@ -27997,7 +27997,7 @@
         <v>128</v>
       </c>
       <c r="D101" s="83">
-        <v>0.79300000000000004</v>
+        <v>2.72</v>
       </c>
       <c r="E101" s="73">
         <v>8</v>
@@ -28062,7 +28062,7 @@
         <v>126</v>
       </c>
       <c r="D102" s="83">
-        <v>0.79300000000000004</v>
+        <v>2.72</v>
       </c>
       <c r="E102" s="73">
         <v>21</v>
@@ -28121,7 +28121,7 @@
         <v>136</v>
       </c>
       <c r="D103" s="83">
-        <v>0.79300000000000004</v>
+        <v>2.72</v>
       </c>
       <c r="E103" s="73">
         <v>40.25</v>
@@ -28265,8 +28265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA127177-25C6-664D-9F19-42DDA7C8C436}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>